<commit_message>
commit3: added pandas logic for weighted averages of sentiment scores
</commit_message>
<xml_diff>
--- a/excel_data/final_df.xlsx
+++ b/excel_data/final_df.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Aggregated Data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="weighted_mean" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,93 +436,1533 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>title</t>
+          <t>link</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>average_Sentiment</t>
+          <t>weighted_sentiment</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>10 from my collection</t>
+          <t>https://reddit.com/r/adidas/comments/1kbqq35/what_yall_think_about_forum2000/</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.2768695652173913</v>
+        <v>0.3341521739130435</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Edison Chen Lunar New Year Superstar - better late than never</t>
+          <t>https://reddit.com/r/adidas/comments/1kbu4gq/adidas_superstar_sakura_celebrates_tokyos_cherry/</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.3901833333333333</v>
+        <v>0.4588</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>First time ordering from GOAT. Very happy 🤍🖤</t>
+          <t>https://reddit.com/r/adidas/comments/1kbwziu/todays_pair_wish_they_would_bring_back_this/</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.3182</v>
+        <v>0.2764875</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Freshly dropped</t>
+          <t>https://reddit.com/r/adidas/comments/1kbyeg6/sporty_rich_handball_spezial/</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1899928571428571</v>
+        <v>0.50008</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Invincibles</t>
+          <t>https://reddit.com/r/adidas/comments/1kbyfwq/just_landed_love_the_colors/</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.6336666666666666</v>
+        <v>0.2346357142857143</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Ordered from Snipes and this is what I received.  I guess keeping the box is out of the question.</t>
+          <t>https://reddit.com/r/adidas/comments/1kbysiy/gazelle_x_clot_halo_ivory/</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.14286</v>
+        <v>0.40962</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>🔥</t>
+          <t>https://reddit.com/r/adidas/comments/1kc18rc/a_price_for_not_checking_twicecan_you_spot_the/</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.3496142857142857</v>
+        <v>-0.0158035294117647</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>🔴 1 of 50: Kith x adidas Predator Megaride.</t>
+          <t>https://reddit.com/r/adidas/comments/1kc2ofu/seriously_good/</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.3392333333333333</v>
+        <v>0.5855</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kc4zrp/running_shoes/</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.37728</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kc852k/its_a_busenitz_vintage_kind_of_day/</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.4400555555555555</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kc8wht/bali/</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.146475</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kcalus/free_sambas/</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.2104818181818182</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kcay98/what_sambas_are_you_wearing_today/</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.27823</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kceqaj/retro_shoe_request/</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.18567</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kcflhf/adidas_in_the_neighborhood/</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kcg20l/identication/</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>-0.4121</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kcgz3o/lets_go_ant/</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0.3798595744680851</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kck0o4/great_shoe_day_brain_dead/</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0.7279</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kck9o1/my_first_pair_of_spezial/</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.4566652173913044</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kcl1yc/are_they_real/</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0.2619454545454545</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kclptc/does_anyone_know_the_name_of_this_trainer_please/</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0.008</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kcqog7/cop_or_drop/</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0.2120822368421053</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kcs43w/super_man_batman_antman_this_is_really_1_of_my/</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>0.34745</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kcsi8r/considering_them_for_everyday_wear_i_live_in/</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>-0.132</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kcun1y/need_help_identifying_these_shoes/</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0.0524875</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kcvpdh/samba_sizing/</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0.389725</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kcxcbj/sizing_help_for_y3_adidas_hoodies_do_they_fit/</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>0.645</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kczhgo/are_10_adidas_tshirts_enough_for_the_gym/</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>0.01909444444444445</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kcztsn/hot_or_not_rate_this_custom/</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>0.09493157894736842</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kd496o/willy_chavarria_x_adidas_originals_jabbar_gress/</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>0.3804999999999999</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kd5fl5/dad_shoes/</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>0.3054222222222223</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kd5l79/adidas_warns_sneakers_will_cost_more_in_the_us_as/</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>0.1283048780487805</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kd6669/upcoming/</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>0.4350333333333333</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kd697j/its_a_campus_day/</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>0.3147</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kd9a6j/adidas_jogging_allround/</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kd9i95/i_may_have_a_problem/</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>0.2212658682634731</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kda7ww/beforeafter/</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>0.3909228813559322</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kde1ci/_/</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>0.3785</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kdej12/samba_madness/</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>0.8300333333333333</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kdenwx/help_identifying_shoes/</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>0.2982</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kdfk1r/my_mom_this_at_the_thrift_and_she_thinks_its_so/</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>0.04636792452830189</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kdgr93/id_please/</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>0.3612</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kdh7zo/2025_is_the_year_of_the_superstars/</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>0.0389125</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kdi0nn/climacool_24_confirmed_app_drawing/</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>0.72255</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kdjjvu/these_pants_ray_have_out_yet/</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kdk2ct/messi_samba_had_to_trim_the_top_border_of_the/</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>0.6486</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kdki08/different_colored_spezials/</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>0.092075</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kdofey/first_pair_of_nmds/</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>0.2489428571428571</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kdqfgg/whats_on_foot_this_weekend_folks/</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>0.5578333333333334</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kdqrqv/samba_og_size_recommandation/</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>0.09336976744186044</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kdrg7u/my_original_shoes/</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>-0.08732857142857142</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kdrum5/do_these_go_with_anyrhing_besides_sportswear/</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>0.1791916666666667</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kdshmw/adidas_in_the_neighborhood/</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>0.8842</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kdt31a/whats_your_take_on_this_color/</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>0.4794666666666667</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kduhk8/are_these_good_for_runningwalking/</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>0.4311428571428571</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kdv2o8/after_the_climacool24_kith_steps_in_with_the/</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>-0.1366</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kdvchx/help_my_sambas_got_wet_and_the_dye_transferred/</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>-0.06381111111111111</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kdvdvm/on_foot_today_on_this_sunny_warm_day/</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>-0.09424285714285714</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kdvhl9/japan_shoes_fit_questions/</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>0.5949555555555555</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kdws5c/more_please/</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>0.74964</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kdx6ve/anyone_have_any_info/</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>0.1225555555555556</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kdxntn/identify_these_shoes_tags_worn_down/</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>0.09030000000000001</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kdxwkv/whats_the_deal_with_stan_smiths_in_2025_leather/</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>0.3428272727272728</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kdyrmt/gazelle_bold/</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>0.56645</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kdz0x6/a_pair_of_shoes_that_dont_exist/</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>0.1745</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kdzn2k/zip_up_jackets_addict/</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>0.6717571428571427</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kdzx19/cant_find_these_shoes_in_larger_sizes_any_chances/</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>0.09866666666666667</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1ke1n1j/which_model_is_this/</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>-0.4341</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1ke2bz8/sw_hemp_gazelles_thoughts/</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>0.3959130434782608</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1ke2tkp/what_even_is_this_gold_coin/</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>0.075875</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1ke3qzr/this_is_a_scam_right/</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>-0.63845</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1ke3su1/my_current_favorite/</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>0.5713999999999999</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1ke4ov1/no_love_for_these/</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>0.43008</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1ke8do3/3ssb_ae1s/</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>-0.128</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1keaqqf/do_you_iron_your_adidas_training_tees_even_though/</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>0.1319133333333334</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1keezsn/a_pleasant_surprise_no_regrets/</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>0.4130444444444445</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1keguyk/help_me_find_adidas_sneakers_from_around_the/</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>0.20725</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kehtju/adidas_handball_spezial/</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>0.6124000000000001</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kejaz9/munchen/</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>0.3071234042553191</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kelz6k/the_wall_at_jd_and_footlocker_us/</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>0.32231875</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kemfn1/travelling_to_new_york/</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>0.62085</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kemvhi/help_please_ive_goggled_and_cant_find_anything/</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>0.1358</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kenl12/may_the_fourth_be_with_you/</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>0.5565666666666667</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1keqkdc/any_hikers_here_use_terrex_skychaser_whats_are/</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>0.6696</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1keqpec/what_color_of_spezial_should_i_buy_next_i_already/</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>0.3925166666666666</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kes3jq/sample_shoes/</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>0.3515</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kesw9l/i_just_got_these/</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>0.4634285714285715</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1ket4h1/anyone_know_if_the_evo_sl_will_restock_again/</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>0.4019</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1keu4hx/zx5000_x_size/</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>0.3294</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1keviy2/got_this_2_years_ago/</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>0.3546818181818182</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kewv4b/getting_these_for_my_birthday_i_think_what_do_you/</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>0.3819484536082474</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kexwmo/does_anyone_know_the_exact_value_of_this_backpack/</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1key3vp/tips_to_clean_shoes/</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>0.4864833333333334</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kezouq/fuck_fuck_fuck_trump/</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>0.2708993055555556</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kf0f92/brain_dead_x_forest_hills/</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>0.3969461538461539</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kf0xj6/adidas_continental_80/</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>0.3512</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kf117t/anyone_know_what_adidas_sneakers_these_are/</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
+        <v>0.03612</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kf3pnu/clot_bring_beaded_detailing_to_the_adidas_stan/</t>
+        </is>
+      </c>
+      <c r="B99" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kf3utn/wore_these_out_today/</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kf52bh/whats_your_favorite/</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>0.507925</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kf87q8/how_do_i_fix_this_from_being_ripped_off/</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kf8cyq/adidas_longevity/</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>0.137208</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kfag60/one_pair_for_each_weekday/</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>0.3173363636363636</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kfc80i/how_do_these_run/</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>0.2946428571428572</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kff28a/matchy/</t>
+        </is>
+      </c>
+      <c r="B106" t="n">
+        <v>0.4019</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kfh71q/any_tips_for_cleaning_up_these_boost_soles_ive/</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>0.324295744680851</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kfivos/wolves_in_4/</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>-0.6486</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kfjejy/why_doesnt_adidas_make_xl_or_2xl_caps/</t>
+        </is>
+      </c>
+      <c r="B109" t="n">
+        <v>-0.4574</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kfk7qq/can_anyone_tell_me_what_shoes_are_these/</t>
+        </is>
+      </c>
+      <c r="B110" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kfl91z/anyone_know_when_the_aristocats_gazelles_release/</t>
+        </is>
+      </c>
+      <c r="B111" t="n">
+        <v>0.2202</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kfmiau/what_old_adidas_model_is_this_and_is_it_a/</t>
+        </is>
+      </c>
+      <c r="B112" t="n">
+        <v>0.1642</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kfoofs/zx8000_mita/</t>
+        </is>
+      </c>
+      <c r="B113" t="n">
+        <v>0.1056</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kfp34f/addidas_style/</t>
+        </is>
+      </c>
+      <c r="B114" t="n">
+        <v>0.006699999999999998</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kft0r1/im_looking_for_this_tracksuit/</t>
+        </is>
+      </c>
+      <c r="B115" t="n">
+        <v>0.1945833333333333</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kfwkwx/gazelle_bold_or_gazelle_indoor/</t>
+        </is>
+      </c>
+      <c r="B116" t="n">
+        <v>0.4479</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kfwth9/how_to_clean_these_stains_off_my_campuses/</t>
+        </is>
+      </c>
+      <c r="B117" t="n">
+        <v>-0.2334333333333334</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kfyh81/balenciaga_x_adidas_bootlegcustomization_or/</t>
+        </is>
+      </c>
+      <c r="B118" t="n">
+        <v>0.02356666666666665</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kg0git/whats_this_a_doing_here/</t>
+        </is>
+      </c>
+      <c r="B119" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kg26kt/anyone_notice_that_academy_and_dicks_back_benched/</t>
+        </is>
+      </c>
+      <c r="B120" t="n">
+        <v>0.3352083333333333</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kg3vnw/freshly_dropped/</t>
+        </is>
+      </c>
+      <c r="B121" t="n">
+        <v>0.08474230769230767</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kg4p4j/willy_chavarria_x_adidas_jabbar_dress_low_drops/</t>
+        </is>
+      </c>
+      <c r="B122" t="n">
+        <v>-0.07235535714285714</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kg7jgt/whats_up_with_these/</t>
+        </is>
+      </c>
+      <c r="B123" t="n">
+        <v>0.6423166666666668</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kg84x0/vl_court_30s_with_2_differences/</t>
+        </is>
+      </c>
+      <c r="B124" t="n">
+        <v>0.6217857142857143</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kg9b3f/edison_chen_lunar_new_year_superstar_better_late/</t>
+        </is>
+      </c>
+      <c r="B125" t="n">
+        <v>0.2060333333333333</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kg9n4a/adidas_refusing_to_refund_me/</t>
+        </is>
+      </c>
+      <c r="B126" t="n">
+        <v>-0.67155</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kgcro1/_/</t>
+        </is>
+      </c>
+      <c r="B127" t="n">
+        <v>0.2759909090909091</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kge2to/invincibles/</t>
+        </is>
+      </c>
+      <c r="B128" t="n">
+        <v>0.5753625</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kge9oi/1_of_50_kith_x_adidas_predator_megaride/</t>
+        </is>
+      </c>
+      <c r="B129" t="n">
+        <v>0.3684684210526316</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kgfngb/10_from_my_collection/</t>
+        </is>
+      </c>
+      <c r="B130" t="n">
+        <v>0.3406785714285714</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kgfou6/ordered_from_snipes_and_this_is_what_i_received_i/</t>
+        </is>
+      </c>
+      <c r="B131" t="n">
+        <v>-0.04874722222222225</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kgfs4f/first_time_ordering_from_goat_very_happy/</t>
+        </is>
+      </c>
+      <c r="B132" t="n">
+        <v>0.30835</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kgg9au/what_do_you_guys_know_about_these/</t>
+        </is>
+      </c>
+      <c r="B133" t="n">
+        <v>-0.63225</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kgif5o/another_pair_of_sambas_love_this_color_way/</t>
+        </is>
+      </c>
+      <c r="B134" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kgl119/having_a_triple_for_the_game_tomorrow/</t>
+        </is>
+      </c>
+      <c r="B135" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kgm1zm/first_pair_of_sambas_half_off_at_nearby_outlet/</t>
+        </is>
+      </c>
+      <c r="B136" t="n">
+        <v>0.5383045454545455</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kgokga/shipping_time_for_an_exchange/</t>
+        </is>
+      </c>
+      <c r="B137" t="n">
+        <v>0.29862</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kgppe1/is_there_a_current_model_similar_to_this_one/</t>
+        </is>
+      </c>
+      <c r="B138" t="n">
+        <v>0.5023</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kgq4vv/zx10000/</t>
+        </is>
+      </c>
+      <c r="B139" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kgw12q/lego_adidas_limited_edition_out_of_100/</t>
+        </is>
+      </c>
+      <c r="B140" t="n">
+        <v>0.2016157894736842</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kgw9xv/vegan_sambas/</t>
+        </is>
+      </c>
+      <c r="B141" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kgxo5h/kith_megarides_on_foot_today/</t>
+        </is>
+      </c>
+      <c r="B142" t="n">
+        <v>-0.1027</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kgyjuw/the_100_thieves_x_adidas_palos_hills_drops_this/</t>
+        </is>
+      </c>
+      <c r="B143" t="n">
+        <v>0.02394999999999999</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kgz1zb/amazing/</t>
+        </is>
+      </c>
+      <c r="B144" t="n">
+        <v>0.1585</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kh05tn/any_love_for_the_samoas/</t>
+        </is>
+      </c>
+      <c r="B145" t="n">
+        <v>0.2801399999999999</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kh1k3t/is_it_just_me_or_does_the_three_sole_bottom_make/</t>
+        </is>
+      </c>
+      <c r="B146" t="n">
+        <v>0.2611470588235295</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kh234n/adidas_torsion_zx_8000_sneakers_red_yellow_black/</t>
+        </is>
+      </c>
+      <c r="B147" t="n">
+        <v>0.17145</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kh2w1e/is_shopsimoncom_a_trusted_site_to_buy_adidas/</t>
+        </is>
+      </c>
+      <c r="B148" t="n">
+        <v>0.03572142857142857</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kh3zuz/id_help/</t>
+        </is>
+      </c>
+      <c r="B149" t="n">
+        <v>0.0258</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kh5lqb/orange_green_or_yellow/</t>
+        </is>
+      </c>
+      <c r="B150" t="n">
+        <v>0.1832107142857143</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kh607b/do_sambas_crumble/</t>
+        </is>
+      </c>
+      <c r="B151" t="n">
+        <v>0.31074</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kh71hy/newest_pair/</t>
+        </is>
+      </c>
+      <c r="B152" t="n">
+        <v>0.71965</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>https://reddit.com/r/adidas/comments/1kh7zat/blue_and_white_gazelle_or_messi_x_samba/</t>
+        </is>
+      </c>
+      <c r="B153" t="n">
+        <v>-0.1366</v>
       </c>
     </row>
   </sheetData>

</xml_diff>